<commit_message>
more more row formatting
</commit_message>
<xml_diff>
--- a/example_models/simple_model.xlsx
+++ b/example_models/simple_model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wescummings/projects/ghqctoolkit/example_models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26748C7F-B1EE-2447-BC81-6879D0D32C9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{394BF042-3409-9941-B288-4AA137637E4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="34560" windowHeight="20200" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -362,16 +362,16 @@
     <t>New Thing</t>
   </si>
   <si>
-    <t>e_2</t>
-  </si>
-  <si>
     <t>time &lt; tc</t>
   </si>
   <si>
-    <t>dose_amount=old_dose</t>
-  </si>
-  <si>
     <t>Reset dose</t>
+  </si>
+  <si>
+    <t>e_3</t>
+  </si>
+  <si>
+    <t>dose_amount!=new_dose</t>
   </si>
 </sst>
 </file>
@@ -1643,7 +1643,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="206" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1691,19 +1691,19 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>108</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="D3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>